<commit_message>
Add k fold pair tests
</commit_message>
<xml_diff>
--- a/testy_parowe.xlsx
+++ b/testy_parowe.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9510" firstSheet="9" activeTab="15"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9510" firstSheet="3" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet" sheetId="1" r:id="rId1"/>
@@ -2689,12 +2689,13 @@
   <dimension ref="A1:S20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M2" sqref="M2:M20"/>
+      <selection activeCell="Q1" sqref="Q1:S14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="13" max="13" width="11.5703125" customWidth="1"/>
+    <col min="18" max="18" width="16.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.25">
@@ -2874,7 +2875,7 @@
         <v>116</v>
       </c>
       <c r="R4" s="1">
-        <v>0.68690476190476191</v>
+        <v>0.70457983193277318</v>
       </c>
       <c r="S4" s="1">
         <v>0.66557422969187674</v>
@@ -2924,7 +2925,7 @@
         <v>117</v>
       </c>
       <c r="R5" s="1">
-        <v>2.7882187733481211E-3</v>
+        <v>1.0529878618113918E-3</v>
       </c>
       <c r="S5" s="1">
         <v>1.1089176411305259E-3</v>
@@ -3024,7 +3025,7 @@
         <v>119</v>
       </c>
       <c r="R7" s="1">
-        <v>-8.2873249776161707E-3</v>
+        <v>0.36792906356288235</v>
       </c>
       <c r="S7" s="1"/>
     </row>
@@ -3168,7 +3169,7 @@
         <v>122</v>
       </c>
       <c r="R10" s="1">
-        <v>1.0764924891336893</v>
+        <v>3.3364407827675242</v>
       </c>
       <c r="S10" s="1"/>
     </row>
@@ -3216,7 +3217,7 @@
         <v>123</v>
       </c>
       <c r="R11" s="1">
-        <v>0.1548577246824579</v>
+        <v>4.3546751014448236E-3</v>
       </c>
       <c r="S11" s="1"/>
     </row>
@@ -3312,7 +3313,7 @@
         <v>125</v>
       </c>
       <c r="R13" s="1">
-        <v>0.3097154493649158</v>
+        <v>8.7093502028896472E-3</v>
       </c>
       <c r="S13" s="1"/>
     </row>
@@ -6403,7 +6404,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="Q25" sqref="O24:Q25"/>
     </sheetView>
   </sheetViews>
@@ -8285,7 +8286,7 @@
   <dimension ref="A1:S20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M2" sqref="M2:M20"/>
+      <selection activeCell="Q1" sqref="Q1:S14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8470,7 +8471,7 @@
         <v>116</v>
       </c>
       <c r="R4" s="1">
-        <v>0.71993431855500822</v>
+        <v>0.7345812807881773</v>
       </c>
       <c r="S4" s="1">
         <v>0.69850574712643687</v>
@@ -8520,7 +8521,7 @@
         <v>117</v>
       </c>
       <c r="R5" s="1">
-        <v>5.6817113245967773E-3</v>
+        <v>9.6163081958904328E-3</v>
       </c>
       <c r="S5" s="1">
         <v>6.9950361436686608E-3</v>
@@ -8620,7 +8621,7 @@
         <v>119</v>
       </c>
       <c r="R7" s="1">
-        <v>0.84644774118267008</v>
+        <v>0.80878447541733556</v>
       </c>
       <c r="S7" s="1"/>
     </row>
@@ -8764,7 +8765,7 @@
         <v>122</v>
       </c>
       <c r="R10" s="1">
-        <v>1.5136089132185806</v>
+        <v>1.9725859349371861</v>
       </c>
       <c r="S10" s="1"/>
     </row>
@@ -8812,7 +8813,7 @@
         <v>123</v>
       </c>
       <c r="R11" s="1">
-        <v>8.2210569948079293E-2</v>
+        <v>4.0004293875832229E-2</v>
       </c>
       <c r="S11" s="1"/>
     </row>
@@ -8908,7 +8909,7 @@
         <v>125</v>
       </c>
       <c r="R13" s="1">
-        <v>0.16442113989615859</v>
+        <v>8.0008587751664459E-2</v>
       </c>
       <c r="S13" s="1"/>
     </row>
@@ -9215,8 +9216,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M2" sqref="M2:M20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Q1" sqref="Q1:S14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9401,7 +9402,7 @@
         <v>116</v>
       </c>
       <c r="R4" s="1">
-        <v>0.55817204301075274</v>
+        <v>0.57827956989247309</v>
       </c>
       <c r="S4" s="1">
         <v>0.53827956989247305</v>
@@ -9451,7 +9452,7 @@
         <v>117</v>
       </c>
       <c r="R5" s="1">
-        <v>5.9093408358063355E-3</v>
+        <v>8.1537493094899893E-3</v>
       </c>
       <c r="S5" s="1">
         <v>9.058259785974028E-3</v>
@@ -9551,7 +9552,7 @@
         <v>119</v>
       </c>
       <c r="R7" s="1">
-        <v>0.81938002760438855</v>
+        <v>0.7465936412302614</v>
       </c>
       <c r="S7" s="1"/>
     </row>
@@ -9695,7 +9696,7 @@
         <v>122</v>
       </c>
       <c r="R10" s="1">
-        <v>1.1527405839782519</v>
+        <v>1.9114073070779845</v>
       </c>
       <c r="S10" s="1"/>
     </row>
@@ -9743,7 +9744,7 @@
         <v>123</v>
       </c>
       <c r="R11" s="1">
-        <v>0.13935682908531569</v>
+        <v>4.4131287115237811E-2</v>
       </c>
       <c r="S11" s="1"/>
     </row>
@@ -9839,7 +9840,7 @@
         <v>125</v>
       </c>
       <c r="R13" s="1">
-        <v>0.27871365817063137</v>
+        <v>8.8262574230475621E-2</v>
       </c>
       <c r="S13" s="1"/>
     </row>

</xml_diff>